<commit_message>
Add unit test, refactor test utilities and update test reference data frames with new budget
</commit_message>
<xml_diff>
--- a/data/tests/reference_dataframes/df_budgeted.xlsx
+++ b/data/tests/reference_dataframes/df_budgeted.xlsx
@@ -549,7 +549,7 @@
         <v>0.001817297286857026</v>
       </c>
       <c r="Q2" t="n">
-        <v>247145.1633569314</v>
+        <v>145383.7829485621</v>
       </c>
     </row>
     <row r="3">
@@ -608,7 +608,7 @@
         <v>0.001665738835013793</v>
       </c>
       <c r="Q3" t="n">
-        <v>224323.8403694909</v>
+        <v>133259.1068011035</v>
       </c>
     </row>
     <row r="4">
@@ -667,7 +667,7 @@
         <v>0.001836318306628823</v>
       </c>
       <c r="Q4" t="n">
-        <v>245201.8341276278</v>
+        <v>146905.4645303058</v>
       </c>
     </row>
     <row r="5">
@@ -726,7 +726,7 @@
         <v>0.002304742839433383</v>
       </c>
       <c r="Q5" t="n">
-        <v>301981.096731724</v>
+        <v>184379.4271546707</v>
       </c>
     </row>
     <row r="6">
@@ -785,7 +785,7 @@
         <v>0.002019464494441086</v>
       </c>
       <c r="Q6" t="n">
-        <v>270451.7048498327</v>
+        <v>161557.1595552869</v>
       </c>
     </row>
     <row r="7">
@@ -844,7 +844,7 @@
         <v>0.001144565884808555</v>
       </c>
       <c r="Q7" t="n">
-        <v>152955.1840340008</v>
+        <v>91565.27078468438</v>
       </c>
     </row>
     <row r="8">
@@ -903,7 +903,7 @@
         <v>0.00308904960074028</v>
       </c>
       <c r="Q8" t="n">
-        <v>420207.8232929966</v>
+        <v>247123.9680592224</v>
       </c>
     </row>
     <row r="9">
@@ -962,7 +962,7 @@
         <v>0.002630538660216249</v>
       </c>
       <c r="Q9" t="n">
-        <v>359193.5141672253</v>
+        <v>210443.0928172999</v>
       </c>
     </row>
     <row r="10">
@@ -1021,7 +1021,7 @@
         <v>0.001021121629309376</v>
       </c>
       <c r="Q10" t="n">
-        <v>136964.6785301848</v>
+        <v>81689.73034475009</v>
       </c>
     </row>
     <row r="11">
@@ -1080,7 +1080,7 @@
         <v>0.003200173773892004</v>
       </c>
       <c r="Q11" t="n">
-        <v>436130.8425313046</v>
+        <v>256013.9019113603</v>
       </c>
     </row>
     <row r="12">
@@ -1139,7 +1139,7 @@
         <v>0.0005623428157551008</v>
       </c>
       <c r="Q12" t="n">
-        <v>77460.03781116173</v>
+        <v>44987.42526040806</v>
       </c>
     </row>
     <row r="13">
@@ -1198,7 +1198,7 @@
         <v>0.002472806256349825</v>
       </c>
       <c r="Q13" t="n">
-        <v>244675.5694717373</v>
+        <v>197824.500507986</v>
       </c>
     </row>
     <row r="14">
@@ -1257,7 +1257,7 @@
         <v>0.001093968165156986</v>
       </c>
       <c r="Q14" t="n">
-        <v>147832.7759154222</v>
+        <v>87517.45321255884</v>
       </c>
     </row>
     <row r="15">
@@ -1316,7 +1316,7 @@
         <v>0.002186277573180444</v>
       </c>
       <c r="Q15" t="n">
-        <v>295128.1792003706</v>
+        <v>174902.2058544355</v>
       </c>
     </row>
     <row r="16">
@@ -1375,7 +1375,7 @@
         <v>0.001067645463849949</v>
       </c>
       <c r="Q16" t="n">
-        <v>148793.8866456891</v>
+        <v>85411.63710799594</v>
       </c>
     </row>
     <row r="17">
@@ -1434,7 +1434,7 @@
         <v>0.00356739370656008</v>
       </c>
       <c r="Q17" t="n">
-        <v>493823.7799560066</v>
+        <v>285391.4965248064</v>
       </c>
     </row>
     <row r="18">
@@ -1493,7 +1493,7 @@
         <v>0.03972383655830358</v>
       </c>
       <c r="Q18" t="n">
-        <v>5700895.695834678</v>
+        <v>3177906.924664286</v>
       </c>
     </row>
     <row r="19">
@@ -1552,7 +1552,7 @@
         <v>0.008280211349789152</v>
       </c>
       <c r="Q19" t="n">
-        <v>1144548.542258413</v>
+        <v>662416.9079831322</v>
       </c>
     </row>
     <row r="20">
@@ -1611,7 +1611,7 @@
         <v>0.002498357007512022</v>
       </c>
       <c r="Q20" t="n">
-        <v>335116.949191585</v>
+        <v>199868.5606009618</v>
       </c>
     </row>
     <row r="21">
@@ -1670,7 +1670,7 @@
         <v>0.0005168485089937681</v>
       </c>
       <c r="Q21" t="n">
-        <v>70345.69219854497</v>
+        <v>41347.88071950145</v>
       </c>
     </row>
     <row r="22">
@@ -1729,7 +1729,7 @@
         <v>0.003166654864345582</v>
       </c>
       <c r="Q22" t="n">
-        <v>436387.560294673</v>
+        <v>253332.3891476466</v>
       </c>
     </row>
     <row r="23">
@@ -1788,7 +1788,7 @@
         <v>0.0006573475852186936</v>
       </c>
       <c r="Q23" t="n">
-        <v>83166.04646239581</v>
+        <v>52587.80681749548</v>
       </c>
     </row>
     <row r="24">
@@ -1847,7 +1847,7 @@
         <v>0.0004678627273963032</v>
       </c>
       <c r="Q24" t="n">
-        <v>60959.78864092194</v>
+        <v>37429.01819170426</v>
       </c>
     </row>
     <row r="25">
@@ -1906,7 +1906,7 @@
         <v>0.004256898597932654</v>
       </c>
       <c r="Q25" t="n">
-        <v>571550.8894288692</v>
+        <v>340551.8878346123</v>
       </c>
     </row>
     <row r="26">
@@ -1965,7 +1965,7 @@
         <v>0.005895056523347588</v>
       </c>
       <c r="Q26" t="n">
-        <v>790853.542478621</v>
+        <v>471604.5218678071</v>
       </c>
     </row>
     <row r="27">
@@ -2024,7 +2024,7 @@
         <v>0.00580957584038938</v>
       </c>
       <c r="Q27" t="n">
-        <v>801548.2291894627</v>
+        <v>464766.0672311505</v>
       </c>
     </row>
     <row r="28">
@@ -2083,7 +2083,7 @@
         <v>0.001861362320089778</v>
       </c>
       <c r="Q28" t="n">
-        <v>246130.8546451144</v>
+        <v>148908.9856071823</v>
       </c>
     </row>
     <row r="29">
@@ -2142,7 +2142,7 @@
         <v>0.0006575235978595854</v>
       </c>
       <c r="Q29" t="n">
-        <v>89984.63784916983</v>
+        <v>52601.88782876683</v>
       </c>
     </row>
     <row r="30">
@@ -2201,7 +2201,7 @@
         <v>0.00171762483047957</v>
       </c>
       <c r="Q30" t="n">
-        <v>233180.490942202</v>
+        <v>137409.9864383656</v>
       </c>
     </row>
     <row r="31">
@@ -2260,7 +2260,7 @@
         <v>0.001308833303946809</v>
       </c>
       <c r="Q31" t="n">
-        <v>176460.7976842085</v>
+        <v>104706.6643157447</v>
       </c>
     </row>
     <row r="32">
@@ -2319,7 +2319,7 @@
         <v>0.002881213640569955</v>
       </c>
       <c r="Q32" t="n">
-        <v>393922.8554848261</v>
+        <v>230497.0912455964</v>
       </c>
     </row>
     <row r="33">
@@ -2378,7 +2378,7 @@
         <v>0.01592174719948963</v>
       </c>
       <c r="Q33" t="n">
-        <v>2239705.08747138</v>
+        <v>1273739.775959171</v>
       </c>
     </row>
     <row r="34">
@@ -2437,7 +2437,7 @@
         <v>0.004294633523246581</v>
       </c>
       <c r="Q34" t="n">
-        <v>581432.0193541727</v>
+        <v>343570.6818597264</v>
       </c>
     </row>
     <row r="35">
@@ -2496,7 +2496,7 @@
         <v>0.002065724802584539</v>
       </c>
       <c r="Q35" t="n">
-        <v>284316.7376220339</v>
+        <v>165257.9842067632</v>
       </c>
     </row>
     <row r="36">
@@ -2555,7 +2555,7 @@
         <v>0.0007243162838621003</v>
       </c>
       <c r="Q36" t="n">
-        <v>98139.21377286066</v>
+        <v>57945.30270896803</v>
       </c>
     </row>
     <row r="37">
@@ -2614,7 +2614,7 @@
         <v>0.0005597592800998497</v>
       </c>
       <c r="Q37" t="n">
-        <v>77434.02999146005</v>
+        <v>44780.74240798798</v>
       </c>
     </row>
     <row r="38">
@@ -2673,7 +2673,7 @@
         <v>0.005838637168200106</v>
       </c>
       <c r="Q38" t="n">
-        <v>778862.81812664</v>
+        <v>467090.9734560084</v>
       </c>
     </row>
     <row r="39">
@@ -2732,7 +2732,7 @@
         <v>0.04542865871231985</v>
       </c>
       <c r="Q39" t="n">
-        <v>6033697.990337575</v>
+        <v>3634292.696985588</v>
       </c>
     </row>
     <row r="40">
@@ -2791,7 +2791,7 @@
         <v>0.001172941890540878</v>
       </c>
       <c r="Q40" t="n">
-        <v>158906.9590800976</v>
+        <v>93835.35124327023</v>
       </c>
     </row>
     <row r="41">
@@ -2850,7 +2850,7 @@
         <v>0.001964004266619108</v>
       </c>
       <c r="Q41" t="n">
-        <v>263724.2766046823</v>
+        <v>157120.3413295286</v>
       </c>
     </row>
     <row r="42">
@@ -2909,7 +2909,7 @@
         <v>0.00464843585090282</v>
       </c>
       <c r="Q42" t="n">
-        <v>625618.9282539564</v>
+        <v>371874.8680722256</v>
       </c>
     </row>
     <row r="43">
@@ -2968,7 +2968,7 @@
         <v>0.002685131307831368</v>
       </c>
       <c r="Q43" t="n">
-        <v>358684.0906984261</v>
+        <v>214810.5046265095</v>
       </c>
     </row>
     <row r="44">
@@ -3027,7 +3027,7 @@
         <v>0.001133779689049032</v>
       </c>
       <c r="Q44" t="n">
-        <v>153025.054577432</v>
+        <v>90702.37512392255</v>
       </c>
     </row>
     <row r="45">
@@ -3086,7 +3086,7 @@
         <v>0.001489567045317554</v>
       </c>
       <c r="Q45" t="n">
-        <v>201884.5831482591</v>
+        <v>119165.3636254044</v>
       </c>
     </row>
     <row r="46">
@@ -3145,7 +3145,7 @@
         <v>0.0003570776293170902</v>
       </c>
       <c r="Q46" t="n">
-        <v>49051.77402682474</v>
+        <v>28566.21034536722</v>
       </c>
     </row>
     <row r="47">
@@ -3204,7 +3204,7 @@
         <v>0.001141523168373136</v>
       </c>
       <c r="Q47" t="n">
-        <v>155346.5571503525</v>
+        <v>91321.85346985086</v>
       </c>
     </row>
     <row r="48">
@@ -3263,7 +3263,7 @@
         <v>0.001154078257254275</v>
       </c>
       <c r="Q48" t="n">
-        <v>153616.6243067491</v>
+        <v>92326.26058034203</v>
       </c>
     </row>
     <row r="49">
@@ -3322,7 +3322,7 @@
         <v>0.0006972957968514095</v>
       </c>
       <c r="Q49" t="n">
-        <v>96019.18491846102</v>
+        <v>55783.66374811276</v>
       </c>
     </row>
     <row r="50">
@@ -3381,7 +3381,7 @@
         <v>0.002029868784447296</v>
       </c>
       <c r="Q50" t="n">
-        <v>271840.5854308812</v>
+        <v>162389.5027557837</v>
       </c>
     </row>
     <row r="51">
@@ -3440,7 +3440,7 @@
         <v>0.000871335277722338</v>
       </c>
       <c r="Q51" t="n">
-        <v>118580.7795880746</v>
+        <v>69706.82221778703</v>
       </c>
     </row>
     <row r="52">
@@ -3499,7 +3499,7 @@
         <v>0.01421526575982146</v>
       </c>
       <c r="Q52" t="n">
-        <v>1881664.553524353</v>
+        <v>1137221.260785717</v>
       </c>
     </row>
     <row r="53">
@@ -3558,7 +3558,7 @@
         <v>0.01438436604802619</v>
       </c>
       <c r="Q53" t="n">
-        <v>1902039.098643999</v>
+        <v>1150749.283842095</v>
       </c>
     </row>
     <row r="54">
@@ -3617,7 +3617,7 @@
         <v>0.001044395569014856</v>
       </c>
       <c r="Q54" t="n">
-        <v>143220.857175083</v>
+        <v>83551.64552118847</v>
       </c>
     </row>
     <row r="55">
@@ -3676,7 +3676,7 @@
         <v>0.002145336220298382</v>
       </c>
       <c r="Q55" t="n">
-        <v>289835.8567995412</v>
+        <v>171626.8976238706</v>
       </c>
     </row>
     <row r="56">
@@ -3735,7 +3735,7 @@
         <v>0.0004285394705719779</v>
       </c>
       <c r="Q56" t="n">
-        <v>59842.04716182915</v>
+        <v>34283.15764575823</v>
       </c>
     </row>
     <row r="57">
@@ -3794,7 +3794,7 @@
         <v>0.002711230307675791</v>
       </c>
       <c r="Q57" t="n">
-        <v>364851.5856184455</v>
+        <v>216898.4246140633</v>
       </c>
     </row>
     <row r="58">
@@ -3853,7 +3853,7 @@
         <v>0.0004567490833429815</v>
       </c>
       <c r="Q58" t="n">
-        <v>61560.06184573705</v>
+        <v>36539.92666743852</v>
       </c>
     </row>
     <row r="59">
@@ -3912,7 +3912,7 @@
         <v>0.0007413653657790313</v>
       </c>
       <c r="Q59" t="n">
-        <v>104798.2005725367</v>
+        <v>59309.22926232251</v>
       </c>
     </row>
     <row r="60">
@@ -3971,7 +3971,7 @@
         <v>0.0004377324887653716</v>
       </c>
       <c r="Q60" t="n">
-        <v>58693.49006496957</v>
+        <v>35018.59910122973</v>
       </c>
     </row>
     <row r="61">
@@ -4030,7 +4030,7 @@
         <v>0.0008974949942096823</v>
       </c>
       <c r="Q61" t="n">
-        <v>119125.9784107052</v>
+        <v>71799.59953677459</v>
       </c>
     </row>
     <row r="62">
@@ -4089,7 +4089,7 @@
         <v>0.001936444666284899</v>
       </c>
       <c r="Q62" t="n">
-        <v>262941.5694257681</v>
+        <v>154915.5733027919</v>
       </c>
     </row>
     <row r="63">
@@ -4148,7 +4148,7 @@
         <v>0.002469334883407298</v>
       </c>
       <c r="Q63" t="n">
-        <v>330202.6597457465</v>
+        <v>197546.7906725838</v>
       </c>
     </row>
     <row r="64">
@@ -4207,7 +4207,7 @@
         <v>0.01045264669179124</v>
       </c>
       <c r="Q64" t="n">
-        <v>1391138.091227351</v>
+        <v>836211.7353432992</v>
       </c>
     </row>
     <row r="65">
@@ -4266,7 +4266,7 @@
         <v>0.001783962643646023</v>
       </c>
       <c r="Q65" t="n">
-        <v>240175.7929522682</v>
+        <v>142717.0114916819</v>
       </c>
     </row>
     <row r="66">
@@ -4325,7 +4325,7 @@
         <v>0.003161467291678838</v>
       </c>
       <c r="Q66" t="n">
-        <v>423889.3328419755</v>
+        <v>252917.3833343071</v>
       </c>
     </row>
     <row r="67">
@@ -4384,7 +4384,7 @@
         <v>0.0009138802083708069</v>
       </c>
       <c r="Q67" t="n">
-        <v>124091.4157436658</v>
+        <v>73110.41666966456</v>
       </c>
     </row>
     <row r="68">
@@ -4443,7 +4443,7 @@
         <v>0.002501667555410517</v>
       </c>
       <c r="Q68" t="n">
-        <v>339303.5431408284</v>
+        <v>200133.4044328413</v>
       </c>
     </row>
     <row r="69">
@@ -4502,7 +4502,7 @@
         <v>0.001822074559533891</v>
       </c>
       <c r="Q69" t="n">
-        <v>243455.8051776339</v>
+        <v>145765.9647627113</v>
       </c>
     </row>
     <row r="70">
@@ -4561,7 +4561,7 @@
         <v>0.0008138354570541359</v>
       </c>
       <c r="Q70" t="n">
-        <v>108576.3725172314</v>
+        <v>65106.83656433087</v>
       </c>
     </row>
     <row r="71">
@@ -4620,7 +4620,7 @@
         <v>0.0009803496565641255</v>
       </c>
       <c r="Q71" t="n">
-        <v>132669.549318436</v>
+        <v>78427.97252513004</v>
       </c>
     </row>
     <row r="72">
@@ -4679,7 +4679,7 @@
         <v>0.0005030333257219096</v>
       </c>
       <c r="Q72" t="n">
-        <v>67496.91517760872</v>
+        <v>40242.66605775277</v>
       </c>
     </row>
     <row r="73">
@@ -4738,7 +4738,7 @@
         <v>0.001159424806927439</v>
       </c>
       <c r="Q73" t="n">
-        <v>157476.6416381783</v>
+        <v>92753.98455419511</v>
       </c>
     </row>
     <row r="74">
@@ -4797,7 +4797,7 @@
         <v>0.001531936714792251</v>
       </c>
       <c r="Q74" t="n">
-        <v>207516.2640159577</v>
+        <v>122554.93718338</v>
       </c>
     </row>
     <row r="75">
@@ -4856,7 +4856,7 @@
         <v>0.001404863390852127</v>
       </c>
       <c r="Q75" t="n">
-        <v>189595.8960347598</v>
+        <v>112389.0712681702</v>
       </c>
     </row>
     <row r="76">
@@ -4915,7 +4915,7 @@
         <v>0.001518968691540898</v>
       </c>
       <c r="Q76" t="n">
-        <v>204241.7609587131</v>
+        <v>121517.4953232718</v>
       </c>
     </row>
     <row r="77">
@@ -4974,7 +4974,7 @@
         <v>0.004233159690120562</v>
       </c>
       <c r="Q77" t="n">
-        <v>589056.5076200694</v>
+        <v>338652.7752096449</v>
       </c>
     </row>
     <row r="78">
@@ -5033,7 +5033,7 @@
         <v>0.004037446572823377</v>
       </c>
       <c r="Q78" t="n">
-        <v>547437.3295522111</v>
+        <v>322995.7258258702</v>
       </c>
     </row>
     <row r="79">
@@ -5092,7 +5092,7 @@
         <v>0.0005295503688357485</v>
       </c>
       <c r="Q79" t="n">
-        <v>72064.26197876653</v>
+        <v>42364.02950685988</v>
       </c>
     </row>
     <row r="80">
@@ -5151,7 +5151,7 @@
         <v>0.0005121960287284226</v>
       </c>
       <c r="Q80" t="n">
-        <v>68571.99199710834</v>
+        <v>40975.6822982738</v>
       </c>
     </row>
     <row r="81">
@@ -5210,7 +5210,7 @@
         <v>0.001086909587397115</v>
       </c>
       <c r="Q81" t="n">
-        <v>143607.9314107036</v>
+        <v>86952.76699176918</v>
       </c>
     </row>
     <row r="82">
@@ -5269,7 +5269,7 @@
         <v>0.001148144551546698</v>
       </c>
       <c r="Q82" t="n">
-        <v>154433.4510519645</v>
+        <v>91851.56412373585</v>
       </c>
     </row>
     <row r="83">
@@ -5328,7 +5328,7 @@
         <v>0.001513376717441684</v>
       </c>
       <c r="Q83" t="n">
-        <v>207650.4556921886</v>
+        <v>121070.1373953347</v>
       </c>
     </row>
     <row r="84">
@@ -5387,7 +5387,7 @@
         <v>0.0007192546869971722</v>
       </c>
       <c r="Q84" t="n">
-        <v>97465.73129551607</v>
+        <v>57540.37495977377</v>
       </c>
     </row>
     <row r="85">
@@ -5446,7 +5446,7 @@
         <v>0.003436250821560314</v>
       </c>
       <c r="Q85" t="n">
-        <v>467349.4578623645</v>
+        <v>274900.0657248251</v>
       </c>
     </row>
     <row r="86">
@@ -5505,7 +5505,7 @@
         <v>0.001681926274453621</v>
       </c>
       <c r="Q86" t="n">
-        <v>216691.5626196677</v>
+        <v>134554.1019562896</v>
       </c>
     </row>
     <row r="87">
@@ -5564,7 +5564,7 @@
         <v>0.00214886528087162</v>
       </c>
       <c r="Q87" t="n">
-        <v>293120.1418677306</v>
+        <v>171909.2224697296</v>
       </c>
     </row>
     <row r="88">
@@ -5623,7 +5623,7 @@
         <v>0.003161123436514209</v>
       </c>
       <c r="Q88" t="n">
-        <v>424141.2394008556</v>
+        <v>252889.8749211367</v>
       </c>
     </row>
     <row r="89">
@@ -5682,7 +5682,7 @@
         <v>0.001399891223150239</v>
       </c>
       <c r="Q89" t="n">
-        <v>189630.003982907</v>
+        <v>111991.2978520191</v>
       </c>
     </row>
     <row r="90">
@@ -5741,7 +5741,7 @@
         <v>0.001312649169440977</v>
       </c>
       <c r="Q90" t="n">
-        <v>178389.708821689</v>
+        <v>105011.9335552782</v>
       </c>
     </row>
     <row r="91">
@@ -5800,7 +5800,7 @@
         <v>0.00763215841282836</v>
       </c>
       <c r="Q91" t="n">
-        <v>1177663.987212121</v>
+        <v>610572.6730262688</v>
       </c>
     </row>
     <row r="92">
@@ -5859,7 +5859,7 @@
         <v>0.0008321105079369366</v>
       </c>
       <c r="Q92" t="n">
-        <v>112208.0554169658</v>
+        <v>66568.84063495493</v>
       </c>
     </row>
     <row r="93">
@@ -5918,7 +5918,7 @@
         <v>0.002989008214963819</v>
       </c>
       <c r="Q93" t="n">
-        <v>403889.7849617982</v>
+        <v>239120.6571971056</v>
       </c>
     </row>
     <row r="94">
@@ -5977,7 +5977,7 @@
         <v>0.001889176236999589</v>
       </c>
       <c r="Q94" t="n">
-        <v>257901.118062931</v>
+        <v>151134.0989599671</v>
       </c>
     </row>
     <row r="95">
@@ -6036,7 +6036,7 @@
         <v>0.002520223272343713</v>
       </c>
       <c r="Q95" t="n">
-        <v>267363.2963034592</v>
+        <v>201617.861787497</v>
       </c>
     </row>
     <row r="96">
@@ -6095,7 +6095,7 @@
         <v>0.001155915996869457</v>
       </c>
       <c r="Q96" t="n">
-        <v>156981.7113722326</v>
+        <v>92473.27974955652</v>
       </c>
     </row>
     <row r="97">
@@ -6154,7 +6154,7 @@
         <v>0.0009965393384547708</v>
       </c>
       <c r="Q97" t="n">
-        <v>134504.3650616487</v>
+        <v>79723.14707638166</v>
       </c>
     </row>
     <row r="98">
@@ -6213,7 +6213,7 @@
         <v>0.001679490976498856</v>
       </c>
       <c r="Q98" t="n">
-        <v>226267.9735264019</v>
+        <v>134359.2781199085</v>
       </c>
     </row>
     <row r="99">
@@ -6272,7 +6272,7 @@
         <v>0.00180937461093097</v>
       </c>
       <c r="Q99" t="n">
-        <v>256578.5129860895</v>
+        <v>144749.9688744776</v>
       </c>
     </row>
     <row r="100">
@@ -6331,7 +6331,7 @@
         <v>0.001601783422047201</v>
       </c>
       <c r="Q100" t="n">
-        <v>214206.2353114811</v>
+        <v>128142.6737637761</v>
       </c>
     </row>
     <row r="101">
@@ -6390,7 +6390,7 @@
         <v>0.0008708804858058227</v>
       </c>
       <c r="Q101" t="n">
-        <v>117892.358720456</v>
+        <v>69670.43886446582</v>
       </c>
     </row>
     <row r="102">
@@ -6449,7 +6449,7 @@
         <v>0.001567311296117248</v>
       </c>
       <c r="Q102" t="n">
-        <v>208414.364049016</v>
+        <v>125384.9036893798</v>
       </c>
     </row>
     <row r="103">
@@ -6508,7 +6508,7 @@
         <v>0.001501044438971856</v>
       </c>
       <c r="Q103" t="n">
-        <v>204329.3459052367</v>
+        <v>120083.5551177485</v>
       </c>
     </row>
     <row r="104">
@@ -6567,7 +6567,7 @@
         <v>0.001831315710421644</v>
       </c>
       <c r="Q104" t="n">
-        <v>246338.9314361708</v>
+        <v>146505.2568337315</v>
       </c>
     </row>
     <row r="105">
@@ -6626,7 +6626,7 @@
         <v>0.001957926861279432</v>
       </c>
       <c r="Q105" t="n">
-        <v>264495.3139462289</v>
+        <v>156634.1489023546</v>
       </c>
     </row>
     <row r="106">
@@ -6685,7 +6685,7 @@
         <v>0.00196339284364623</v>
       </c>
       <c r="Q106" t="n">
-        <v>262195.2062054134</v>
+        <v>157071.4274916984</v>
       </c>
     </row>
     <row r="107">
@@ -6744,7 +6744,7 @@
         <v>0.0008597629255633812</v>
       </c>
       <c r="Q107" t="n">
-        <v>115047.4221855047</v>
+        <v>68781.0340450705</v>
       </c>
     </row>
     <row r="108">
@@ -6803,7 +6803,7 @@
         <v>0.001217000026673815</v>
       </c>
       <c r="Q108" t="n">
-        <v>163788.6933100769</v>
+        <v>97360.00213390522</v>
       </c>
     </row>
     <row r="109">
@@ -6862,7 +6862,7 @@
         <v>0.00116545426799963</v>
       </c>
       <c r="Q109" t="n">
-        <v>156330.9230529008</v>
+        <v>93236.34143997041</v>
       </c>
     </row>
     <row r="110">
@@ -6921,7 +6921,7 @@
         <v>0.001241832438797608</v>
       </c>
       <c r="Q110" t="n">
-        <v>167929.772776612</v>
+        <v>99346.59510380862</v>
       </c>
     </row>
     <row r="111">
@@ -6980,7 +6980,7 @@
         <v>0.001067769463145919</v>
       </c>
       <c r="Q111" t="n">
-        <v>146019.8608699967</v>
+        <v>85421.55705167355</v>
       </c>
     </row>
     <row r="112">
@@ -7039,7 +7039,7 @@
         <v>0.001983788354276362</v>
       </c>
       <c r="Q112" t="n">
-        <v>267483.7041459332</v>
+        <v>158703.0683421089</v>
       </c>
     </row>
     <row r="113">
@@ -7098,7 +7098,7 @@
         <v>0.0009029352293954702</v>
       </c>
       <c r="Q113" t="n">
-        <v>121529.1574920152</v>
+        <v>72234.81835163762</v>
       </c>
     </row>
     <row r="114">
@@ -7157,7 +7157,7 @@
         <v>0.001304900044675372</v>
       </c>
       <c r="Q114" t="n">
-        <v>170823.3742315589</v>
+        <v>104392.0035740297</v>
       </c>
     </row>
     <row r="115">
@@ -7216,7 +7216,7 @@
         <v>0.001843524993079872</v>
       </c>
       <c r="Q115" t="n">
-        <v>246317.0842660917</v>
+        <v>147481.9994463898</v>
       </c>
     </row>
     <row r="116">
@@ -7275,7 +7275,7 @@
         <v>0.001353482657060236</v>
       </c>
       <c r="Q116" t="n">
-        <v>184226.3918356017</v>
+        <v>108278.6125648189</v>
       </c>
     </row>
     <row r="117">
@@ -7334,7 +7334,7 @@
         <v>0.001170163917454738</v>
       </c>
       <c r="Q117" t="n">
-        <v>157951.4218387205</v>
+        <v>93613.11339637902</v>
       </c>
     </row>
     <row r="118">
@@ -7393,7 +7393,7 @@
         <v>0.02139629566208408</v>
       </c>
       <c r="Q118" t="n">
-        <v>2966994.719202132</v>
+        <v>1711703.652966726</v>
       </c>
     </row>
     <row r="119">
@@ -7452,7 +7452,7 @@
         <v>0.004237746131639047</v>
       </c>
       <c r="Q119" t="n">
-        <v>581576.4716238779</v>
+        <v>339019.6905311237</v>
       </c>
     </row>
     <row r="120">
@@ -7511,7 +7511,7 @@
         <v>0.005312227451524204</v>
       </c>
       <c r="Q120" t="n">
-        <v>702533.6905447156</v>
+        <v>424978.1961219363</v>
       </c>
     </row>
     <row r="121">
@@ -7570,7 +7570,7 @@
         <v>0.0115113444785527</v>
       </c>
       <c r="Q121" t="n">
-        <v>1523598.288942204</v>
+        <v>920907.5582842161</v>
       </c>
     </row>
     <row r="122">
@@ -7629,7 +7629,7 @@
         <v>0.005840376377244891</v>
       </c>
       <c r="Q122" t="n">
-        <v>751568.8713977905</v>
+        <v>467230.1101795913</v>
       </c>
     </row>
     <row r="123">
@@ -7688,7 +7688,7 @@
         <v>0.004876471990470352</v>
       </c>
       <c r="Q123" t="n">
-        <v>622628.4349130868</v>
+        <v>390117.7592376281</v>
       </c>
     </row>
     <row r="124">
@@ -7747,7 +7747,7 @@
         <v>0.001855249309422685</v>
       </c>
       <c r="Q124" t="n">
-        <v>251876.8358028303</v>
+        <v>148419.9447538148</v>
       </c>
     </row>
     <row r="125">
@@ -7806,7 +7806,7 @@
         <v>0.00206155320882464</v>
       </c>
       <c r="Q125" t="n">
-        <v>277415.4295098539</v>
+        <v>164924.2567059712</v>
       </c>
     </row>
     <row r="126">
@@ -7865,7 +7865,7 @@
         <v>0.005748882860687417</v>
       </c>
       <c r="Q126" t="n">
-        <v>781068.159309941</v>
+        <v>459910.6288549934</v>
       </c>
     </row>
     <row r="127">
@@ -7924,7 +7924,7 @@
         <v>0.001186507686421581</v>
       </c>
       <c r="Q127" t="n">
-        <v>159324.729815182</v>
+        <v>94920.61491372646</v>
       </c>
     </row>
     <row r="128">
@@ -7983,7 +7983,7 @@
         <v>0.003719262465483231</v>
       </c>
       <c r="Q128" t="n">
-        <v>511874.8602651283</v>
+        <v>297540.9972386585</v>
       </c>
     </row>
     <row r="129">
@@ -8042,7 +8042,7 @@
         <v>0.004873477557135424</v>
       </c>
       <c r="Q129" t="n">
-        <v>653884.4121280201</v>
+        <v>389878.2045708339</v>
       </c>
     </row>
     <row r="130">
@@ -8101,7 +8101,7 @@
         <v>0.001122218481263758</v>
       </c>
       <c r="Q130" t="n">
-        <v>147688.7006514539</v>
+        <v>89777.47850110068</v>
       </c>
     </row>
     <row r="131">
@@ -8160,7 +8160,7 @@
         <v>0.008753381759547686</v>
       </c>
       <c r="Q131" t="n">
-        <v>1164228.613872419</v>
+        <v>700270.5407638149</v>
       </c>
     </row>
     <row r="132">
@@ -8219,7 +8219,7 @@
         <v>0.002361360619774268</v>
       </c>
       <c r="Q132" t="n">
-        <v>324070.116242425</v>
+        <v>188908.8495819414</v>
       </c>
     </row>
     <row r="133">
@@ -8278,7 +8278,7 @@
         <v>0.0041048872259737</v>
       </c>
       <c r="Q133" t="n">
-        <v>546804.8357906442</v>
+        <v>328390.9780778961</v>
       </c>
     </row>
     <row r="134">
@@ -8337,7 +8337,7 @@
         <v>0.005276368613614226</v>
       </c>
       <c r="Q134" t="n">
-        <v>705286.6984683875</v>
+        <v>422109.4890891381</v>
       </c>
     </row>
     <row r="135">
@@ -8396,7 +8396,7 @@
         <v>0.004809788330170053</v>
       </c>
       <c r="Q135" t="n">
-        <v>646691.224046309</v>
+        <v>384783.0664136042</v>
       </c>
     </row>
     <row r="136">
@@ -8455,7 +8455,7 @@
         <v>0.003567378454299041</v>
       </c>
       <c r="Q136" t="n">
-        <v>474764.0872677579</v>
+        <v>285390.2763439232</v>
       </c>
     </row>
     <row r="137">
@@ -8514,7 +8514,7 @@
         <v>0.001197085888761505</v>
       </c>
       <c r="Q137" t="n">
-        <v>160812.1813071571</v>
+        <v>95766.8711009204</v>
       </c>
     </row>
     <row r="138">
@@ -8573,7 +8573,7 @@
         <v>0.0007602625965489766</v>
       </c>
       <c r="Q138" t="n">
-        <v>104043.3104882471</v>
+        <v>60821.00772391813</v>
       </c>
     </row>
     <row r="139">
@@ -8632,7 +8632,7 @@
         <v>0.02486255150827902</v>
       </c>
       <c r="Q139" t="n">
-        <v>3172258.645318243</v>
+        <v>1989004.120662322</v>
       </c>
     </row>
     <row r="140">
@@ -8691,7 +8691,7 @@
         <v>0.001043515029310916</v>
       </c>
       <c r="Q140" t="n">
-        <v>140825.5614113242</v>
+        <v>83481.20234487329</v>
       </c>
     </row>
     <row r="141">
@@ -8750,7 +8750,7 @@
         <v>0.001017053757486885</v>
       </c>
       <c r="Q141" t="n">
-        <v>134385.0824309742</v>
+        <v>81364.30059895081</v>
       </c>
     </row>
     <row r="142">
@@ -8809,7 +8809,7 @@
         <v>0.000760267638314175</v>
       </c>
       <c r="Q142" t="n">
-        <v>101828.994823302</v>
+        <v>60821.41106513399</v>
       </c>
     </row>
     <row r="143">
@@ -8868,7 +8868,7 @@
         <v>0.002230387128889872</v>
       </c>
       <c r="Q143" t="n">
-        <v>302143.2841115479</v>
+        <v>178430.9703111897</v>
       </c>
     </row>
     <row r="144">
@@ -8927,7 +8927,7 @@
         <v>0.001983993862711113</v>
       </c>
       <c r="Q144" t="n">
-        <v>262084.7216137404</v>
+        <v>158719.5090168891</v>
       </c>
     </row>
     <row r="145">
@@ -8986,7 +8986,7 @@
         <v>0.0003557294766729387</v>
       </c>
       <c r="Q145" t="n">
-        <v>47901.84798541918</v>
+        <v>28458.3581338351</v>
       </c>
     </row>
     <row r="146">
@@ -9045,7 +9045,7 @@
         <v>0.0005678893663827722</v>
       </c>
       <c r="Q146" t="n">
-        <v>75570.55212113338</v>
+        <v>45431.14931062178</v>
       </c>
     </row>
     <row r="147">
@@ -9104,7 +9104,7 @@
         <v>0.003582442261439812</v>
       </c>
       <c r="Q147" t="n">
-        <v>468479.933669228</v>
+        <v>286595.3809151849</v>
       </c>
     </row>
     <row r="148">
@@ -9163,7 +9163,7 @@
         <v>0.001829881254890868</v>
       </c>
       <c r="Q148" t="n">
-        <v>249231.6444631163</v>
+        <v>146390.5003912694</v>
       </c>
     </row>
     <row r="149">
@@ -9222,7 +9222,7 @@
         <v>0.001237426190980556</v>
       </c>
       <c r="Q149" t="n">
-        <v>166108.0478932824</v>
+        <v>98994.09527844447</v>
       </c>
     </row>
     <row r="150">
@@ -9281,7 +9281,7 @@
         <v>0.001077718585374689</v>
       </c>
       <c r="Q150" t="n">
-        <v>142783.2334120561</v>
+        <v>86217.48682997515</v>
       </c>
     </row>
     <row r="151">
@@ -9340,7 +9340,7 @@
         <v>0.0006208155622324399</v>
       </c>
       <c r="Q151" t="n">
-        <v>83143.54393066929</v>
+        <v>49665.24497859519</v>
       </c>
     </row>
     <row r="152">
@@ -9399,7 +9399,7 @@
         <v>0.000459008149391624</v>
       </c>
       <c r="Q152" t="n">
-        <v>63236.97896763238</v>
+        <v>36720.65195132992</v>
       </c>
     </row>
     <row r="153">
@@ -9458,7 +9458,7 @@
         <v>0.0005416204188954966</v>
       </c>
       <c r="Q153" t="n">
-        <v>74294.66723556802</v>
+        <v>43329.63351163972</v>
       </c>
     </row>
     <row r="154">
@@ -9517,7 +9517,7 @@
         <v>0.0006433399124889881</v>
       </c>
       <c r="Q154" t="n">
-        <v>86822.30476310666</v>
+        <v>51467.19299911905</v>
       </c>
     </row>
     <row r="155">
@@ -9576,7 +9576,7 @@
         <v>0.002524694348322168</v>
       </c>
       <c r="Q155" t="n">
-        <v>334121.1441917019</v>
+        <v>201975.5478657734</v>
       </c>
     </row>
     <row r="156">
@@ -9635,7 +9635,7 @@
         <v>0.001597242526046882</v>
       </c>
       <c r="Q156" t="n">
-        <v>216629.644329496</v>
+        <v>127779.4020837506</v>
       </c>
     </row>
     <row r="157">
@@ -9694,7 +9694,7 @@
         <v>0.0007757492495547471</v>
       </c>
       <c r="Q157" t="n">
-        <v>104398.9437282748</v>
+        <v>62059.93996437977</v>
       </c>
     </row>
     <row r="158">
@@ -9753,7 +9753,7 @@
         <v>0.001199251773829936</v>
       </c>
       <c r="Q158" t="n">
-        <v>158827.9380033125</v>
+        <v>95940.14190639487</v>
       </c>
     </row>
     <row r="159">
@@ -9812,7 +9812,7 @@
         <v>0.001897923772236326</v>
       </c>
       <c r="Q159" t="n">
-        <v>255380.5493948239</v>
+        <v>151833.9017789061</v>
       </c>
     </row>
     <row r="160">
@@ -9871,7 +9871,7 @@
         <v>0.0008086240104021197</v>
       </c>
       <c r="Q160" t="n">
-        <v>106562.3558559282</v>
+        <v>64689.92083216958</v>
       </c>
     </row>
     <row r="161">
@@ -9930,7 +9930,7 @@
         <v>0.0006171292970345113</v>
       </c>
       <c r="Q161" t="n">
-        <v>83755.16457795711</v>
+        <v>49370.3437627609</v>
       </c>
     </row>
     <row r="162">
@@ -9989,7 +9989,7 @@
         <v>0.001833139993873211</v>
       </c>
       <c r="Q162" t="n">
-        <v>247456.2116418687</v>
+        <v>146651.1995098569</v>
       </c>
     </row>
     <row r="163">
@@ -10048,7 +10048,7 @@
         <v>0.00277698513340199</v>
       </c>
       <c r="Q163" t="n">
-        <v>370976.0717694542</v>
+        <v>222158.8106721592</v>
       </c>
     </row>
     <row r="164">
@@ -10107,7 +10107,7 @@
         <v>0.0005453929922393095</v>
       </c>
       <c r="Q164" t="n">
-        <v>74552.68647055642</v>
+        <v>43631.43937914476</v>
       </c>
     </row>
     <row r="165">
@@ -10166,7 +10166,7 @@
         <v>0.0007403210427373493</v>
       </c>
       <c r="Q165" t="n">
-        <v>100170.5747145313</v>
+        <v>59225.68341898794</v>
       </c>
     </row>
     <row r="166">
@@ -10225,7 +10225,7 @@
         <v>0.05693059278144348</v>
       </c>
       <c r="Q166" t="n">
-        <v>7634496.073078411</v>
+        <v>4554447.422515479</v>
       </c>
     </row>
     <row r="167">
@@ -10284,7 +10284,7 @@
         <v>0.003912027433648353</v>
       </c>
       <c r="Q167" t="n">
-        <v>529609.528525708</v>
+        <v>312962.1946918682</v>
       </c>
     </row>
     <row r="168">
@@ -10343,7 +10343,7 @@
         <v>0.002608848414391513</v>
       </c>
       <c r="Q168" t="n">
-        <v>348803.9805251056</v>
+        <v>208707.8731513211</v>
       </c>
     </row>
     <row r="169">
@@ -10402,7 +10402,7 @@
         <v>0.04052003777305175</v>
       </c>
       <c r="Q169" t="n">
-        <v>5144433.414425908</v>
+        <v>3241603.02184414</v>
       </c>
     </row>
     <row r="170">
@@ -10461,7 +10461,7 @@
         <v>0.00537933233290127</v>
       </c>
       <c r="Q170" t="n">
-        <v>692550.6052067459</v>
+        <v>430346.5866321016</v>
       </c>
     </row>
     <row r="171">
@@ -10520,7 +10520,7 @@
         <v>0.0013378399703215</v>
       </c>
       <c r="Q171" t="n">
-        <v>174265.6829700395</v>
+        <v>107027.19762572</v>
       </c>
     </row>
     <row r="172">
@@ -10579,7 +10579,7 @@
         <v>0.006223743025660157</v>
       </c>
       <c r="Q172" t="n">
-        <v>813503.5055980828</v>
+        <v>497899.4420528126</v>
       </c>
     </row>
     <row r="173">
@@ -10638,7 +10638,7 @@
         <v>0.002241567395852229</v>
       </c>
       <c r="Q173" t="n">
-        <v>303844.828759003</v>
+        <v>179325.3916681783</v>
       </c>
     </row>
     <row r="174">
@@ -10697,7 +10697,7 @@
         <v>0.001884809979605606</v>
       </c>
       <c r="Q174" t="n">
-        <v>256742.9272610076</v>
+        <v>150784.7983684485</v>
       </c>
     </row>
     <row r="175">
@@ -10756,7 +10756,7 @@
         <v>0.005944940725609168</v>
       </c>
       <c r="Q175" t="n">
-        <v>799174.9850426876</v>
+        <v>475595.2580487335</v>
       </c>
     </row>
     <row r="176">
@@ -10815,7 +10815,7 @@
         <v>0.002220393516041905</v>
       </c>
       <c r="Q176" t="n">
-        <v>293964.7165802349</v>
+        <v>177631.4812833524</v>
       </c>
     </row>
     <row r="177">
@@ -10874,7 +10874,7 @@
         <v>0.0008247205723315692</v>
       </c>
       <c r="Q177" t="n">
-        <v>110643.2107383611</v>
+        <v>65977.64578652554</v>
       </c>
     </row>
     <row r="178">
@@ -10933,7 +10933,7 @@
         <v>0.002360158344500542</v>
       </c>
       <c r="Q178" t="n">
-        <v>316870.9809092662</v>
+        <v>188812.6675600433</v>
       </c>
     </row>
     <row r="179">
@@ -10992,7 +10992,7 @@
         <v>0.003356014299049457</v>
       </c>
       <c r="Q179" t="n">
-        <v>453729.1290361366</v>
+        <v>268481.1439239566</v>
       </c>
     </row>
     <row r="180">
@@ -11051,7 +11051,7 @@
         <v>0.001469239514340694</v>
       </c>
       <c r="Q180" t="n">
-        <v>198427.4503789352</v>
+        <v>117539.1611472555</v>
       </c>
     </row>
     <row r="181">
@@ -11110,7 +11110,7 @@
         <v>0.003442184552458758</v>
       </c>
       <c r="Q181" t="n">
-        <v>453204.1538472508</v>
+        <v>275374.7641967006</v>
       </c>
     </row>
     <row r="182">
@@ -11169,7 +11169,7 @@
         <v>0.0005423175380327664</v>
       </c>
       <c r="Q182" t="n">
-        <v>73381.37910511739</v>
+        <v>43385.40304262131</v>
       </c>
     </row>
     <row r="183">
@@ -11228,7 +11228,7 @@
         <v>0.0007611284158550852</v>
       </c>
       <c r="Q183" t="n">
-        <v>96417.81621854927</v>
+        <v>60890.27326840682</v>
       </c>
     </row>
     <row r="184">
@@ -11287,7 +11287,7 @@
         <v>0.002262887666201576</v>
       </c>
       <c r="Q184" t="n">
-        <v>306385.9877034468</v>
+        <v>181031.013296126</v>
       </c>
     </row>
     <row r="185">
@@ -11346,7 +11346,7 @@
         <v>0.0009289856332974494</v>
       </c>
       <c r="Q185" t="n">
-        <v>122236.9080666696</v>
+        <v>74318.85066379595</v>
       </c>
     </row>
     <row r="186">
@@ -11405,7 +11405,7 @@
         <v>0.001369042460753558</v>
       </c>
       <c r="Q186" t="n">
-        <v>178004.0812430928</v>
+        <v>109523.3968602846</v>
       </c>
     </row>
     <row r="187">
@@ -11464,7 +11464,7 @@
         <v>0.001103264843745238</v>
       </c>
       <c r="Q187" t="n">
-        <v>148970.2096739916</v>
+        <v>88261.18749961903</v>
       </c>
     </row>
     <row r="188">
@@ -11523,7 +11523,7 @@
         <v>0.0003021968606560507</v>
       </c>
       <c r="Q188" t="n">
-        <v>40092.39761859392</v>
+        <v>24175.74885248406</v>
       </c>
     </row>
     <row r="189">
@@ -11582,7 +11582,7 @@
         <v>0.001760740375979932</v>
       </c>
       <c r="Q189" t="n">
-        <v>238416.2017137393</v>
+        <v>140859.2300783946</v>
       </c>
     </row>
     <row r="190">
@@ -11641,7 +11641,7 @@
         <v>0.0001939685664231891</v>
       </c>
       <c r="Q190" t="n">
-        <v>26395.05723259055</v>
+        <v>15517.48531385513</v>
       </c>
     </row>
     <row r="191">
@@ -11700,7 +11700,7 @@
         <v>0.0005280319657610728</v>
       </c>
       <c r="Q191" t="n">
-        <v>71024.79759772167</v>
+        <v>42242.55726088582</v>
       </c>
     </row>
     <row r="192">
@@ -11759,7 +11759,7 @@
         <v>0.001500418876568506</v>
       </c>
       <c r="Q192" t="n">
-        <v>202800.8718575965</v>
+        <v>120033.5101254805</v>
       </c>
     </row>
     <row r="193">
@@ -11818,7 +11818,7 @@
         <v>0.001068794155957276</v>
       </c>
       <c r="Q193" t="n">
-        <v>143315.923022774</v>
+        <v>85503.53247658211</v>
       </c>
     </row>
     <row r="194">
@@ -11877,7 +11877,7 @@
         <v>0.001500284350806054</v>
       </c>
       <c r="Q194" t="n">
-        <v>204432.2480122928</v>
+        <v>120022.7480644843</v>
       </c>
     </row>
     <row r="195">
@@ -11936,7 +11936,7 @@
         <v>0.005394573899258836</v>
       </c>
       <c r="Q195" t="n">
-        <v>721037.178253989</v>
+        <v>431565.9119407068</v>
       </c>
     </row>
     <row r="196">
@@ -11995,7 +11995,7 @@
         <v>0.002312591881275071</v>
       </c>
       <c r="Q196" t="n">
-        <v>312275.4249763596</v>
+        <v>185007.3505020057</v>
       </c>
     </row>
     <row r="197">
@@ -12054,7 +12054,7 @@
         <v>0.001131644615251878</v>
       </c>
       <c r="Q197" t="n">
-        <v>153305.9551048636</v>
+        <v>90531.56922015025</v>
       </c>
     </row>
     <row r="198">
@@ -12113,7 +12113,7 @@
         <v>0.001994571557870599</v>
       </c>
       <c r="Q198" t="n">
-        <v>259388.8440357325</v>
+        <v>159565.7246296479</v>
       </c>
     </row>
     <row r="199">
@@ -12172,7 +12172,7 @@
         <v>0.001697804360589208</v>
       </c>
       <c r="Q199" t="n">
-        <v>226499.1253491299</v>
+        <v>135824.3488471367</v>
       </c>
     </row>
     <row r="200">
@@ -12231,7 +12231,7 @@
         <v>0.001580744191056661</v>
       </c>
       <c r="Q200" t="n">
-        <v>205878.0886698917</v>
+        <v>126459.5352845329</v>
       </c>
     </row>
     <row r="201">
@@ -12290,7 +12290,7 @@
         <v>0.0007002335944597116</v>
       </c>
       <c r="Q201" t="n">
-        <v>93786.81503462786</v>
+        <v>56018.68755677692</v>
       </c>
     </row>
     <row r="202">
@@ -12349,7 +12349,7 @@
         <v>0.0008996456109327002</v>
       </c>
       <c r="Q202" t="n">
-        <v>121752.5175757719</v>
+        <v>71971.64887461602</v>
       </c>
     </row>
     <row r="203">
@@ -12408,7 +12408,7 @@
         <v>0.001292897156561276</v>
       </c>
       <c r="Q203" t="n">
-        <v>174221.4910517174</v>
+        <v>103431.772524902</v>
       </c>
     </row>
     <row r="204">
@@ -12467,7 +12467,7 @@
         <v>0.001423475585731401</v>
       </c>
       <c r="Q204" t="n">
-        <v>189706.4157299323</v>
+        <v>113878.0468585121</v>
       </c>
     </row>
     <row r="205">
@@ -12526,7 +12526,7 @@
         <v>0.0009216820344822707</v>
       </c>
       <c r="Q205" t="n">
-        <v>124836.8967502285</v>
+        <v>73734.56275858165</v>
       </c>
     </row>
     <row r="206">
@@ -12585,7 +12585,7 @@
         <v>0.0007722192695630574</v>
       </c>
       <c r="Q206" t="n">
-        <v>105708.2972170437</v>
+        <v>61777.54156504459</v>
       </c>
     </row>
     <row r="207">
@@ -12644,7 +12644,7 @@
         <v>0.008664836486503581</v>
       </c>
       <c r="Q207" t="n">
-        <v>1151711.49255899</v>
+        <v>693186.9189202865</v>
       </c>
     </row>
     <row r="208">
@@ -12703,7 +12703,7 @@
         <v>0.004911830024584645</v>
       </c>
       <c r="Q208" t="n">
-        <v>643060.1510274226</v>
+        <v>392946.4019667716</v>
       </c>
     </row>
     <row r="209">
@@ -12762,7 +12762,7 @@
         <v>0.001971925450515455</v>
       </c>
       <c r="Q209" t="n">
-        <v>252164.2633662703</v>
+        <v>157754.0360412364</v>
       </c>
     </row>
     <row r="210">
@@ -12821,7 +12821,7 @@
         <v>0.00239177298854863</v>
       </c>
       <c r="Q210" t="n">
-        <v>325508.5810591416</v>
+        <v>191341.8390838904</v>
       </c>
     </row>
     <row r="211">
@@ -12880,7 +12880,7 @@
         <v>0.0006042324140428512</v>
       </c>
       <c r="Q211" t="n">
-        <v>82425.7922486469</v>
+        <v>48338.5931234281</v>
       </c>
     </row>
     <row r="212">
@@ -12939,7 +12939,7 @@
         <v>0.002060295098963118</v>
       </c>
       <c r="Q212" t="n">
-        <v>275071.1167113583</v>
+        <v>164823.6079170495</v>
       </c>
     </row>
     <row r="213">
@@ -12998,7 +12998,7 @@
         <v>0.0004508693743335193</v>
       </c>
       <c r="Q213" t="n">
-        <v>60900.82796080848</v>
+        <v>36069.54994668154</v>
       </c>
     </row>
     <row r="214">
@@ -13057,7 +13057,7 @@
         <v>0.0007654354856513818</v>
       </c>
       <c r="Q214" t="n">
-        <v>104576.9884322526</v>
+        <v>61234.83885211054</v>
       </c>
     </row>
     <row r="215">
@@ -13116,7 +13116,7 @@
         <v>0.0009234745711839432</v>
       </c>
       <c r="Q215" t="n">
-        <v>123320.2996594641</v>
+        <v>73877.96569471546</v>
       </c>
     </row>
     <row r="216">
@@ -13175,7 +13175,7 @@
         <v>0.0009583649381750175</v>
       </c>
       <c r="Q216" t="n">
-        <v>127355.7734220977</v>
+        <v>76669.19505400139</v>
       </c>
     </row>
     <row r="217">
@@ -13234,7 +13234,7 @@
         <v>0.0004535350209598059</v>
       </c>
       <c r="Q217" t="n">
-        <v>61504.7740954349</v>
+        <v>36282.80167678447</v>
       </c>
     </row>
     <row r="218">
@@ -13293,7 +13293,7 @@
         <v>0.01181339439065587</v>
       </c>
       <c r="Q218" t="n">
-        <v>1575531.964607163</v>
+        <v>945071.5512524698</v>
       </c>
     </row>
     <row r="219">
@@ -13352,7 +13352,7 @@
         <v>0.001753566854898081</v>
       </c>
       <c r="Q219" t="n">
-        <v>235433.8257281825</v>
+        <v>140285.3483918465</v>
       </c>
     </row>
     <row r="220">
@@ -13411,7 +13411,7 @@
         <v>0.0009693991056932592</v>
       </c>
       <c r="Q220" t="n">
-        <v>133180.939290774</v>
+        <v>77551.92845546073</v>
       </c>
     </row>
     <row r="221">
@@ -13470,7 +13470,7 @@
         <v>0.007387635292697838</v>
       </c>
       <c r="Q221" t="n">
-        <v>985416.6663023185</v>
+        <v>591010.823415827</v>
       </c>
     </row>
     <row r="222">
@@ -13529,7 +13529,7 @@
         <v>0.001273444443682394</v>
       </c>
       <c r="Q222" t="n">
-        <v>170293.2964906559</v>
+        <v>101875.5554945915</v>
       </c>
     </row>
     <row r="223">
@@ -13588,7 +13588,7 @@
         <v>0.000733558336780494</v>
       </c>
       <c r="Q223" t="n">
-        <v>100142.1497522887</v>
+        <v>58684.66694243952</v>
       </c>
     </row>
     <row r="224">
@@ -13647,7 +13647,7 @@
         <v>0.001130598438236649</v>
       </c>
       <c r="Q224" t="n">
-        <v>153211.6344535373</v>
+        <v>90447.87505893195</v>
       </c>
     </row>
     <row r="225">
@@ -13706,7 +13706,7 @@
         <v>0.000707421080007713</v>
       </c>
       <c r="Q225" t="n">
-        <v>96662.60346979361</v>
+        <v>56593.68640061704</v>
       </c>
     </row>
     <row r="226">
@@ -13765,7 +13765,7 @@
         <v>0.0009911606724103562</v>
       </c>
       <c r="Q226" t="n">
-        <v>133432.5002584934</v>
+        <v>79292.85379282849</v>
       </c>
     </row>
     <row r="227">
@@ -13824,7 +13824,7 @@
         <v>0.004650676136539707</v>
       </c>
       <c r="Q227" t="n">
-        <v>614482.8157716661</v>
+        <v>372054.0909231766</v>
       </c>
     </row>
     <row r="228">
@@ -13883,7 +13883,7 @@
         <v>0.0005254519279265105</v>
       </c>
       <c r="Q228" t="n">
-        <v>71070.56596158179</v>
+        <v>42036.15423412084</v>
       </c>
     </row>
     <row r="229">
@@ -13942,7 +13942,7 @@
         <v>0.0009780776805339397</v>
       </c>
       <c r="Q229" t="n">
-        <v>132928.9266476404</v>
+        <v>78246.21444271518</v>
       </c>
     </row>
     <row r="230">
@@ -14001,7 +14001,7 @@
         <v>0.001832115326320267</v>
       </c>
       <c r="Q230" t="n">
-        <v>240380.4957773879</v>
+        <v>146569.2261056214</v>
       </c>
     </row>
     <row r="231">
@@ -14060,7 +14060,7 @@
         <v>0.001710596576404693</v>
       </c>
       <c r="Q231" t="n">
-        <v>232403.9106946046</v>
+        <v>136847.7261123755</v>
       </c>
     </row>
     <row r="232">
@@ -14119,7 +14119,7 @@
         <v>0.002817748790437033</v>
       </c>
       <c r="Q232" t="n">
-        <v>384792.3746267828</v>
+        <v>225419.9032349627</v>
       </c>
     </row>
     <row r="233">
@@ -14178,7 +14178,7 @@
         <v>0.01015366627476874</v>
       </c>
       <c r="Q233" t="n">
-        <v>1351323.168963144</v>
+        <v>812293.3019814988</v>
       </c>
     </row>
     <row r="234">
@@ -14237,7 +14237,7 @@
         <v>0.0008874858826806296</v>
       </c>
       <c r="Q234" t="n">
-        <v>120172.298039337</v>
+        <v>70998.87061445037</v>
       </c>
     </row>
     <row r="235">
@@ -14296,7 +14296,7 @@
         <v>0.001470991386499588</v>
       </c>
       <c r="Q235" t="n">
-        <v>191276.8536787552</v>
+        <v>117679.3109199671</v>
       </c>
     </row>
     <row r="236">
@@ -14355,7 +14355,7 @@
         <v>0.005493295329701335</v>
       </c>
       <c r="Q236" t="n">
-        <v>726189.3124248311</v>
+        <v>439463.6263761068</v>
       </c>
     </row>
     <row r="237">
@@ -14414,7 +14414,7 @@
         <v>0.001588405571892004</v>
       </c>
       <c r="Q237" t="n">
-        <v>224780.2710528358</v>
+        <v>127072.4457513603</v>
       </c>
     </row>
     <row r="238">
@@ -14473,7 +14473,7 @@
         <v>0.000461769482021606</v>
       </c>
       <c r="Q238" t="n">
-        <v>64172.35250201692</v>
+        <v>36941.55856172848</v>
       </c>
     </row>
     <row r="239">
@@ -14532,7 +14532,7 @@
         <v>0.002558492712608028</v>
       </c>
       <c r="Q239" t="n">
-        <v>346804.1917571712</v>
+        <v>204679.4170086423</v>
       </c>
     </row>
     <row r="240">
@@ -14591,7 +14591,7 @@
         <v>0.0008507649365982675</v>
       </c>
       <c r="Q240" t="n">
-        <v>116321.3017711454</v>
+        <v>68061.1949278614</v>
       </c>
     </row>
     <row r="241">
@@ -14650,7 +14650,7 @@
         <v>0.001159956797932879</v>
       </c>
       <c r="Q241" t="n">
-        <v>157967.9768645057</v>
+        <v>92796.54383463028</v>
       </c>
     </row>
     <row r="242">
@@ -14709,7 +14709,7 @@
         <v>0.001937536666818158</v>
       </c>
       <c r="Q242" t="n">
-        <v>267949.8453320551</v>
+        <v>155002.9333454527</v>
       </c>
     </row>
     <row r="243">
@@ -14768,7 +14768,7 @@
         <v>0.006522837433883357</v>
       </c>
       <c r="Q243" t="n">
-        <v>873268.9673063888</v>
+        <v>521826.9947106686</v>
       </c>
     </row>
     <row r="244">
@@ -14827,7 +14827,7 @@
         <v>0.005477225529228742</v>
       </c>
       <c r="Q244" t="n">
-        <v>762739.1925758101</v>
+        <v>438178.0423382994</v>
       </c>
     </row>
     <row r="245">
@@ -14886,7 +14886,7 @@
         <v>0.003089644530073325</v>
       </c>
       <c r="Q245" t="n">
-        <v>428416.2281988044</v>
+        <v>247171.562405866</v>
       </c>
     </row>
     <row r="246">
@@ -14945,7 +14945,7 @@
         <v>0.002239895027108364</v>
       </c>
       <c r="Q246" t="n">
-        <v>297315.1550483857</v>
+        <v>179191.6021686691</v>
       </c>
     </row>
     <row r="247">
@@ -15004,7 +15004,7 @@
         <v>0.003507102332947191</v>
       </c>
       <c r="Q247" t="n">
-        <v>477917.4820056036</v>
+        <v>280568.1866357753</v>
       </c>
     </row>
     <row r="248">
@@ -15063,7 +15063,7 @@
         <v>0.001698973044614883</v>
       </c>
       <c r="Q248" t="n">
-        <v>224609.8458791505</v>
+        <v>135917.8435691906</v>
       </c>
     </row>
     <row r="249">
@@ -15122,7 +15122,7 @@
         <v>0.002464311510834945</v>
       </c>
       <c r="Q249" t="n">
-        <v>338811.9983600656</v>
+        <v>197144.9208667956</v>
       </c>
     </row>
     <row r="250">
@@ -15181,7 +15181,7 @@
         <v>0.001765784237834408</v>
       </c>
       <c r="Q250" t="n">
-        <v>240401.1954736552</v>
+        <v>141262.7390267526</v>
       </c>
     </row>
     <row r="251">
@@ -15240,7 +15240,7 @@
         <v>0.01418165573295038</v>
       </c>
       <c r="Q251" t="n">
-        <v>1911954.178886447</v>
+        <v>1134532.45863603</v>
       </c>
     </row>
     <row r="252">
@@ -15299,7 +15299,7 @@
         <v>0.002298497902919928</v>
       </c>
       <c r="Q252" t="n">
-        <v>308311.0712690359</v>
+        <v>183879.8322335942</v>
       </c>
     </row>
     <row r="253">
@@ -15358,7 +15358,7 @@
         <v>0.001717389198877933</v>
       </c>
       <c r="Q253" t="n">
-        <v>235787.4446527106</v>
+        <v>137391.1359102346</v>
       </c>
     </row>
     <row r="254">
@@ -15417,7 +15417,7 @@
         <v>0.006624085423940447</v>
       </c>
       <c r="Q254" t="n">
-        <v>838430.4602672361</v>
+        <v>529926.8339152357</v>
       </c>
     </row>
     <row r="255">
@@ -15476,7 +15476,7 @@
         <v>0.0007490857586488546</v>
       </c>
       <c r="Q255" t="n">
-        <v>103583.2593318951</v>
+        <v>59926.86069190837</v>
       </c>
     </row>
     <row r="256">
@@ -15535,7 +15535,7 @@
         <v>0.0008907870033550639</v>
       </c>
       <c r="Q256" t="n">
-        <v>123527.3683339623</v>
+        <v>71262.96026840512</v>
       </c>
     </row>
     <row r="257">
@@ -15594,7 +15594,7 @@
         <v>0.001272683073936978</v>
       </c>
       <c r="Q257" t="n">
-        <v>176653.2563410381</v>
+        <v>101814.6459149582</v>
       </c>
     </row>
     <row r="258">
@@ -15653,7 +15653,7 @@
         <v>0.001401091162258754</v>
       </c>
       <c r="Q258" t="n">
-        <v>192595.2959771958</v>
+        <v>112087.2929807003</v>
       </c>
     </row>
     <row r="259">
@@ -15712,7 +15712,7 @@
         <v>0.0009886087610828471</v>
       </c>
       <c r="Q259" t="n">
-        <v>140807.2947873191</v>
+        <v>79088.70088662778</v>
       </c>
     </row>
     <row r="260">
@@ -15771,7 +15771,7 @@
         <v>0.0009983867301605377</v>
       </c>
       <c r="Q260" t="n">
-        <v>141139.9308796213</v>
+        <v>79870.93841284301</v>
       </c>
     </row>
     <row r="261">
@@ -15830,7 +15830,7 @@
         <v>0.001614220917389839</v>
       </c>
       <c r="Q261" t="n">
-        <v>233054.1890721892</v>
+        <v>129137.6733911871</v>
       </c>
     </row>
     <row r="262">
@@ -15889,7 +15889,7 @@
         <v>0.003188055945164142</v>
       </c>
       <c r="Q262" t="n">
-        <v>446721.2242599948</v>
+        <v>255044.4756131314</v>
       </c>
     </row>
     <row r="263">
@@ -15948,7 +15948,7 @@
         <v>0.0009535230436518724</v>
       </c>
       <c r="Q263" t="n">
-        <v>128202.8493080052</v>
+        <v>76281.8434921498</v>
       </c>
     </row>
     <row r="264">
@@ -16007,7 +16007,7 @@
         <v>0.0003247392901723099</v>
       </c>
       <c r="Q264" t="n">
-        <v>43689.40685654828</v>
+        <v>25979.14321378479</v>
       </c>
     </row>
     <row r="265">
@@ -16066,7 +16066,7 @@
         <v>0.0007678656026757138</v>
       </c>
       <c r="Q265" t="n">
-        <v>103302.0169116549</v>
+        <v>61429.2482140571</v>
       </c>
     </row>
     <row r="266">
@@ -16125,7 +16125,7 @@
         <v>0.001107196854031422</v>
       </c>
       <c r="Q266" t="n">
-        <v>150668.1281382905</v>
+        <v>88575.74832251375</v>
       </c>
     </row>
     <row r="267">
@@ -16184,7 +16184,7 @@
         <v>0.0004697989914882315</v>
       </c>
       <c r="Q267" t="n">
-        <v>64492.20220673714</v>
+        <v>37583.91931905852</v>
       </c>
     </row>
     <row r="268">
@@ -16243,7 +16243,7 @@
         <v>0.0002724521587726608</v>
       </c>
       <c r="Q268" t="n">
-        <v>36625.47985317479</v>
+        <v>21796.17270181286</v>
       </c>
     </row>
     <row r="269">
@@ -16302,7 +16302,7 @@
         <v>0.0008115892742299446</v>
       </c>
       <c r="Q269" t="n">
-        <v>108829.7993131865</v>
+        <v>64927.14193839557</v>
       </c>
     </row>
     <row r="270">
@@ -16361,7 +16361,7 @@
         <v>0.0003996878051144359</v>
       </c>
       <c r="Q270" t="n">
-        <v>52554.84262074949</v>
+        <v>31975.02440915487</v>
       </c>
     </row>
     <row r="271">
@@ -16420,7 +16420,7 @@
         <v>0.000306950398385526</v>
       </c>
       <c r="Q271" t="n">
-        <v>40869.77325016441</v>
+        <v>24556.03187084208</v>
       </c>
     </row>
     <row r="272">
@@ -16479,7 +16479,7 @@
         <v>0.0004969635597261394</v>
       </c>
       <c r="Q272" t="n">
-        <v>66810.9133206798</v>
+        <v>39757.08477809115</v>
       </c>
     </row>
     <row r="273">
@@ -16538,7 +16538,7 @@
         <v>0.0007778884592076378</v>
       </c>
       <c r="Q273" t="n">
-        <v>104252.9097604178</v>
+        <v>62231.07673661102</v>
       </c>
     </row>
     <row r="274">
@@ -16597,7 +16597,7 @@
         <v>0.0005950056686361185</v>
       </c>
       <c r="Q274" t="n">
-        <v>79549.40896300184</v>
+        <v>47600.45349088948</v>
       </c>
     </row>
     <row r="275">
@@ -16656,7 +16656,7 @@
         <v>0.00841895718759467</v>
       </c>
       <c r="Q275" t="n">
-        <v>1139245.854449314</v>
+        <v>673516.5750075736</v>
       </c>
     </row>
     <row r="276">
@@ -16715,7 +16715,7 @@
         <v>0.001597683205024184</v>
       </c>
       <c r="Q276" t="n">
-        <v>218591.4334679544</v>
+        <v>127814.6564019347</v>
       </c>
     </row>
     <row r="277">
@@ -16774,7 +16774,7 @@
         <v>0.01322821380326685</v>
       </c>
       <c r="Q277" t="n">
-        <v>1751763.76803178</v>
+        <v>1058257.104261348</v>
       </c>
     </row>
     <row r="278">
@@ -16833,7 +16833,7 @@
         <v>0.0009873366361483919</v>
       </c>
       <c r="Q278" t="n">
-        <v>131523.1254896938</v>
+        <v>78986.93089187135</v>
       </c>
     </row>
     <row r="279">
@@ -16892,7 +16892,7 @@
         <v>0.0003433098349006814</v>
       </c>
       <c r="Q279" t="n">
-        <v>46619.97327137084</v>
+        <v>27464.78679205451</v>
       </c>
     </row>
     <row r="280">
@@ -16951,7 +16951,7 @@
         <v>0.0009283568301179773</v>
       </c>
       <c r="Q280" t="n">
-        <v>125929.4070211662</v>
+        <v>74268.54640943818</v>
       </c>
     </row>
     <row r="281">
@@ -17010,7 +17010,7 @@
         <v>0.000685707088134955</v>
       </c>
       <c r="Q281" t="n">
-        <v>91528.46801517415</v>
+        <v>54856.5670507964</v>
       </c>
     </row>
     <row r="282">
@@ -17069,7 +17069,7 @@
         <v>0.001670978465143304</v>
       </c>
       <c r="Q282" t="n">
-        <v>219251.054970049</v>
+        <v>133678.2772114643</v>
       </c>
     </row>
     <row r="283">
@@ -17128,7 +17128,7 @@
         <v>0.0004426596296122681</v>
       </c>
       <c r="Q283" t="n">
-        <v>59855.09319964288</v>
+        <v>35412.77036898145</v>
       </c>
     </row>
     <row r="284">
@@ -17187,7 +17187,7 @@
         <v>0.001058489539757707</v>
       </c>
       <c r="Q284" t="n">
-        <v>118255.1698494273</v>
+        <v>84679.16318061655</v>
       </c>
     </row>
     <row r="285">
@@ -17246,7 +17246,7 @@
         <v>0.01025488690570703</v>
       </c>
       <c r="Q285" t="n">
-        <v>1364018.572021165</v>
+        <v>820390.9524565622</v>
       </c>
     </row>
     <row r="286">
@@ -17305,7 +17305,7 @@
         <v>0.0006432746106877039</v>
       </c>
       <c r="Q286" t="n">
-        <v>86349.72915399286</v>
+        <v>51461.9688550163</v>
       </c>
     </row>
     <row r="287">
@@ -17364,7 +17364,7 @@
         <v>0.08771339019431752</v>
       </c>
       <c r="Q287" t="n">
-        <v>11501248.71649638</v>
+        <v>7017071.215545402</v>
       </c>
     </row>
     <row r="288">
@@ -17423,7 +17423,7 @@
         <v>0.00359910010861389</v>
       </c>
       <c r="Q288" t="n">
-        <v>477809.5568764473</v>
+        <v>287928.0086891112</v>
       </c>
     </row>
     <row r="289">
@@ -17482,7 +17482,7 @@
         <v>0.002729897205858486</v>
       </c>
       <c r="Q289" t="n">
-        <v>346437.6352697146</v>
+        <v>218391.7764686789</v>
       </c>
     </row>
     <row r="290">
@@ -17541,7 +17541,7 @@
         <v>0.0007507623333720762</v>
       </c>
       <c r="Q290" t="n">
-        <v>100933.6381041236</v>
+        <v>60060.9866697661</v>
       </c>
     </row>
     <row r="291">
@@ -17600,7 +17600,7 @@
         <v>0.01787386893149022</v>
       </c>
       <c r="Q291" t="n">
-        <v>2352943.613406683</v>
+        <v>1429909.514519218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>